<commit_message>
add error of each measurements
</commit_message>
<xml_diff>
--- a/Experiments/Ellipsometry/data.xlsx
+++ b/Experiments/Ellipsometry/data.xlsx
@@ -19,12 +19,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
-    <t>thickness</t>
+    <t>Temperature</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>temperature</t>
+    <t>Thickness</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Error</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -350,10 +355,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B22"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -361,180 +366,246 @@
     <col min="1" max="1" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>70</v>
       </c>
       <c r="B2">
         <v>121.63</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2">
+        <v>1.7999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>75</v>
       </c>
       <c r="B3">
         <v>121.78</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3">
+        <v>2.1999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>80</v>
       </c>
       <c r="B4">
         <v>121.95</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C4">
+        <v>1.7999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>85</v>
       </c>
       <c r="B5">
         <v>122.15</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C5">
+        <v>2.1000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>90</v>
       </c>
       <c r="B6">
         <v>122.27</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C6">
+        <v>2.1999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>95</v>
       </c>
       <c r="B7">
         <v>122.47</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C7">
+        <v>3.2000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>100</v>
       </c>
       <c r="B8">
         <v>122.54</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C8">
+        <v>2.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>105</v>
       </c>
       <c r="B9">
         <v>122.63</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C9">
+        <v>2.1999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>110</v>
       </c>
       <c r="B10">
         <v>122.98</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C10">
+        <v>3.9E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>115</v>
       </c>
       <c r="B11">
         <v>123.09</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C11">
+        <v>3.5000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>120</v>
       </c>
       <c r="B12">
         <v>123.42</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C12">
+        <v>2.9000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>125</v>
       </c>
       <c r="B13">
         <v>123.59</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C13">
+        <v>3.2000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>130</v>
       </c>
       <c r="B14">
         <v>123.98</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C14">
+        <v>4.7E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>135</v>
       </c>
       <c r="B15">
         <v>124.45</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C15">
+        <v>3.9E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>140</v>
       </c>
       <c r="B16">
         <v>124.88</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C16">
+        <v>5.0999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>145</v>
       </c>
       <c r="B17">
         <v>125.25</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C17">
+        <v>4.9000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>150</v>
       </c>
       <c r="B18">
         <v>125.54</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C18">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>155</v>
       </c>
       <c r="B19">
         <v>125.98</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C19">
+        <v>5.5E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>160</v>
       </c>
       <c r="B20">
         <v>126.44</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C20">
+        <v>4.3999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>165</v>
       </c>
       <c r="B21">
         <v>126.7</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C21">
+        <v>5.7000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>170</v>
       </c>
       <c r="B22">
         <v>127.1</v>
+      </c>
+      <c r="C22">
+        <v>6.0999999999999999E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>